<commit_message>
Created standardized cargo plate format
Also created generic driver for these cargo plates

Fixed old plates so that they were updated. New
ones can be found in the "used-cargo-plates"
folder. Generic driver is currently just floating
in the GUI folder, and not implemented in the
main code yet. Will integrate it soon (hopefully
tomorrow). But in the meantime, it seems able to
import plates from a standard excel file.
</commit_message>
<xml_diff>
--- a/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/GUI/used-cargo-plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE63492D-9C3D-4A72-82C5-3F3235BC0572}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C8A2EE-2228-49D1-B5E3-69B412054AB8}"/>
   <bookViews>
-    <workbookView xWindow="15102" yWindow="0" windowWidth="8016" windowHeight="13758" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2562" yWindow="1962" windowWidth="8094" windowHeight="12438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
     <sheet name="Names" sheetId="2" r:id="rId2"/>
     <sheet name="Descriptions" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="167">
-  <si>
-    <t>new_cargo_strands</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="168">
   <si>
     <t>1</t>
   </si>
@@ -273,132 +283,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>antiBart_h2_cargo_handle_2</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_3</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_8</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_9</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_14</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_15</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_20</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_21</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_26</t>
-  </si>
-  <si>
-    <t>antiBart_h2_cargo_handle_27</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_5</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_6</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_11</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_12</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_17</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_18</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_23</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_24</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_29</t>
-  </si>
-  <si>
-    <t>antiEdna_h2_cargo_handle_30</t>
-  </si>
-  <si>
-    <t>10mer-antiSmithers_h2_cargo_handle_4</t>
-  </si>
-  <si>
-    <t>10mer-antiQuimby_h2_cargo_handle_7</t>
-  </si>
-  <si>
-    <t>10mer-antiPatty_h2_cargo_handle_10</t>
-  </si>
-  <si>
-    <t>10mer-antiMarge_h2_cargo_handle_13</t>
-  </si>
-  <si>
-    <t>10mer-antiSmithers_h2_cargo_handle_14</t>
-  </si>
-  <si>
-    <t>10mer-antiLisa_h2_cargo_handle_16</t>
-  </si>
-  <si>
-    <t>10mer-antiQuimby_h2_cargo_handle_17</t>
-  </si>
-  <si>
-    <t>10mer-antiKrusty_h2_cargo_handle_19</t>
-  </si>
-  <si>
-    <t>10mer-antiPatty_h2_cargo_handle_20</t>
-  </si>
-  <si>
-    <t>10mer-antiHomer_h2_cargo_handle_22</t>
-  </si>
-  <si>
-    <t>10mer-antiMarge_h2_cargo_handle_23</t>
-  </si>
-  <si>
-    <t>10mer-antiLisa_h2_cargo_handle_26</t>
-  </si>
-  <si>
-    <t>10mer-antiKrusty_h2_cargo_handle_29</t>
-  </si>
-  <si>
-    <t>10mer-antiHomer_h2_cargo_handle_32</t>
-  </si>
-  <si>
-    <t>10mer-Homer_h5_cargo_handle_1</t>
-  </si>
-  <si>
-    <t>10mer-Krusty_h5_cargo_handle_6</t>
-  </si>
-  <si>
-    <t>10mer-Lisa_h5_cargo_handle_11</t>
-  </si>
-  <si>
-    <t>10mer-Marge_h5_cargo_handle_16</t>
-  </si>
-  <si>
-    <t>10mer-Patty_h5_cargo_handle_21</t>
-  </si>
-  <si>
-    <t>10mer-Quimby_h5_cargo_handle_26</t>
-  </si>
-  <si>
-    <t>10mer-Smithers_h5_cargo_handle_31</t>
-  </si>
-  <si>
-    <t>biotin_anchor</t>
-  </si>
-  <si>
     <t>h2 attachment for slat position 2, with the antiBart cargo strand.</t>
   </si>
   <si>
@@ -523,13 +407,145 @@
   </si>
   <si>
     <t>Complement for antiNelson, with biotin attached.</t>
+  </si>
+  <si>
+    <t>P3518</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos2</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos3</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos8</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos9</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos14</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos15</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos20</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos21</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos26</t>
+  </si>
+  <si>
+    <t>antiBart_id1_h2_pos27</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos5</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos6</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos11</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos12</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos17</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos18</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos23</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos24</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos29</t>
+  </si>
+  <si>
+    <t>antiEdna_id2_h2_pos30</t>
+  </si>
+  <si>
+    <t>antiSmithers_id3_h2_pos4_10mer</t>
+  </si>
+  <si>
+    <t>antiSmithers_id3_h2_pos14_10mer</t>
+  </si>
+  <si>
+    <t>antiQuimby_id4_h2_pos7_10mer</t>
+  </si>
+  <si>
+    <t>antiPatty_id5_h2_pos10_10mer</t>
+  </si>
+  <si>
+    <t>antiMarge_id6_h2_pos13_10mer</t>
+  </si>
+  <si>
+    <t>antiLisa_id7_h2_pos16_10mer</t>
+  </si>
+  <si>
+    <t>antiQuimby_jd4_h2_pos17_10mer</t>
+  </si>
+  <si>
+    <t>antiKrusty_id8_h2_pos19_10mer</t>
+  </si>
+  <si>
+    <t>antiPatty_id5_h2_pos20_10mer</t>
+  </si>
+  <si>
+    <t>antiHomer_id9_h2_pos22_10mer</t>
+  </si>
+  <si>
+    <t>antiMarge_id6_h2_pos23_10mer</t>
+  </si>
+  <si>
+    <t>antiLisa_id7_h2_pos26_10mer</t>
+  </si>
+  <si>
+    <t>antiKrusty_id8_h2_pos29_10mer</t>
+  </si>
+  <si>
+    <t>antiHomer_id9_h2_pos32_10mer</t>
+  </si>
+  <si>
+    <t>Homer_id10_h5_pos1_10mer</t>
+  </si>
+  <si>
+    <t>Krusty_id11_h5_pos6_10mer</t>
+  </si>
+  <si>
+    <t>Lisa_id12_h5_pos11_10mer</t>
+  </si>
+  <si>
+    <t>Marge_id13_h5_pos16_10mer</t>
+  </si>
+  <si>
+    <t>Patty_id14_h5_pos21_10mer</t>
+  </si>
+  <si>
+    <t>Quimby_id15_h5_pos26_10mer</t>
+  </si>
+  <si>
+    <t>Smithers_id16_id3_h5_pos31_10mer</t>
+  </si>
+  <si>
+    <t>biotin-anchor_id17</t>
+  </si>
+  <si>
+    <t>(\w+)_id(\d+)_h(\d+)_pos(\d+)(?:_(\w+))?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +557,12 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -578,9 +600,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -598,6 +624,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -887,291 +917,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0"/>
+    <sheetView zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>38</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>39</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>41</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>42</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>43</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>44</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>45</v>
-      </c>
-      <c r="K3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>51</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>52</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>54</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>55</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>56</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>57</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>58</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>59</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>60</v>
-      </c>
-      <c r="O4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>63</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>64</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>65</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>66</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>67</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>68</v>
-      </c>
-      <c r="H5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1183,292 +1215,641 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="31.15625" customWidth="1"/>
+    <col min="2" max="15" width="30.1015625" customWidth="1"/>
+    <col min="16" max="25" width="6" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H2" t="s">
-        <v>89</v>
-      </c>
-      <c r="I2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" t="s">
-        <v>91</v>
-      </c>
-      <c r="K2" t="s">
-        <v>92</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" t="s">
-        <v>100</v>
-      </c>
-      <c r="J3" t="s">
-        <v>101</v>
-      </c>
-      <c r="K3" t="s">
-        <v>102</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" t="s">
-        <v>109</v>
-      </c>
-      <c r="I4" t="s">
-        <v>110</v>
-      </c>
-      <c r="J4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" t="s">
-        <v>112</v>
-      </c>
-      <c r="L4" t="s">
-        <v>113</v>
-      </c>
-      <c r="M4" t="s">
-        <v>114</v>
-      </c>
-      <c r="N4" t="s">
-        <v>115</v>
-      </c>
-      <c r="O4" t="s">
-        <v>116</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>120</v>
-      </c>
-      <c r="F5" t="s">
-        <v>121</v>
-      </c>
-      <c r="G5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H5" t="s">
-        <v>123</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>124</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>73</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>75</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>76</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>77</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>78</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>79</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>80</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1479,291 +1860,293 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>128</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>86</v>
       </c>
       <c r="G2" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="H2" t="s">
-        <v>131</v>
+        <v>88</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>133</v>
+        <v>90</v>
       </c>
       <c r="K2" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>136</v>
+        <v>93</v>
       </c>
       <c r="D3" t="s">
-        <v>137</v>
+        <v>94</v>
       </c>
       <c r="E3" t="s">
-        <v>138</v>
+        <v>95</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>98</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="J3" t="s">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="K3" t="s">
-        <v>144</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>148</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="G4" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="H4" t="s">
-        <v>151</v>
+        <v>108</v>
       </c>
       <c r="I4" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="J4" t="s">
-        <v>153</v>
+        <v>110</v>
       </c>
       <c r="K4" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="L4" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="M4" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
       <c r="N4" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="O4" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
       <c r="G5" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
       <c r="H5" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created new GenericPlate for cargo import.
Now it is actually part of the plate system, not
a standalone function.
</commit_message>
<xml_diff>
--- a/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/GUI/used-cargo-plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1C8A2EE-2228-49D1-B5E3-69B412054AB8}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5C4674-00C8-4EAA-B4F3-BD5F2D2EA9FE}"/>
   <bookViews>
-    <workbookView xWindow="2562" yWindow="1962" windowWidth="8094" windowHeight="12438" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
@@ -412,133 +412,133 @@
     <t>P3518</t>
   </si>
   <si>
-    <t>antiBart_id1_h2_pos2</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos3</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos8</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos9</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos14</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos15</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos20</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos21</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos26</t>
-  </si>
-  <si>
-    <t>antiBart_id1_h2_pos27</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos5</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos6</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos11</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos12</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos17</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos18</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos23</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos24</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos29</t>
-  </si>
-  <si>
-    <t>antiEdna_id2_h2_pos30</t>
-  </si>
-  <si>
-    <t>antiSmithers_id3_h2_pos4_10mer</t>
-  </si>
-  <si>
-    <t>antiSmithers_id3_h2_pos14_10mer</t>
-  </si>
-  <si>
-    <t>antiQuimby_id4_h2_pos7_10mer</t>
-  </si>
-  <si>
-    <t>antiPatty_id5_h2_pos10_10mer</t>
-  </si>
-  <si>
-    <t>antiMarge_id6_h2_pos13_10mer</t>
-  </si>
-  <si>
-    <t>antiLisa_id7_h2_pos16_10mer</t>
-  </si>
-  <si>
-    <t>antiQuimby_jd4_h2_pos17_10mer</t>
-  </si>
-  <si>
-    <t>antiKrusty_id8_h2_pos19_10mer</t>
-  </si>
-  <si>
-    <t>antiPatty_id5_h2_pos20_10mer</t>
-  </si>
-  <si>
-    <t>antiHomer_id9_h2_pos22_10mer</t>
-  </si>
-  <si>
-    <t>antiMarge_id6_h2_pos23_10mer</t>
-  </si>
-  <si>
-    <t>antiLisa_id7_h2_pos26_10mer</t>
-  </si>
-  <si>
-    <t>antiKrusty_id8_h2_pos29_10mer</t>
-  </si>
-  <si>
-    <t>antiHomer_id9_h2_pos32_10mer</t>
-  </si>
-  <si>
-    <t>Homer_id10_h5_pos1_10mer</t>
-  </si>
-  <si>
-    <t>Krusty_id11_h5_pos6_10mer</t>
-  </si>
-  <si>
-    <t>Lisa_id12_h5_pos11_10mer</t>
-  </si>
-  <si>
-    <t>Marge_id13_h5_pos16_10mer</t>
-  </si>
-  <si>
-    <t>Patty_id14_h5_pos21_10mer</t>
-  </si>
-  <si>
-    <t>Quimby_id15_h5_pos26_10mer</t>
-  </si>
-  <si>
-    <t>Smithers_id16_id3_h5_pos31_10mer</t>
-  </si>
-  <si>
     <t>biotin-anchor_id17</t>
   </si>
   <si>
-    <t>(\w+)_id(\d+)_h(\d+)_pos(\d+)(?:_(\w+))?</t>
+    <t>antiBart_h2_pos2</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos3</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos8</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos9</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos14</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos15</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos20</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos21</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos26</t>
+  </si>
+  <si>
+    <t>antiBart_h2_pos27</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos5</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos6</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos11</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos12</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos17</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos18</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos23</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos24</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos29</t>
+  </si>
+  <si>
+    <t>antiEdna_h2_pos30</t>
+  </si>
+  <si>
+    <t>antiSmithers-10mer_h2_pos4</t>
+  </si>
+  <si>
+    <t>antiQuimby-10mer_h2_pos7</t>
+  </si>
+  <si>
+    <t>antiPatty-10mer_h2_pos10</t>
+  </si>
+  <si>
+    <t>antiMarge-10mer_h2_pos13</t>
+  </si>
+  <si>
+    <t>antiSmithers-10mer_h2_pos14</t>
+  </si>
+  <si>
+    <t>antiLisa-10mer_h2_pos16</t>
+  </si>
+  <si>
+    <t>antiQuimby-10mer_h2_pos17</t>
+  </si>
+  <si>
+    <t>antiKrusty-10mer_h2_pos19</t>
+  </si>
+  <si>
+    <t>antiPatty-10mer_h2_pos20</t>
+  </si>
+  <si>
+    <t>antiHomer-10mer_h2_pos22</t>
+  </si>
+  <si>
+    <t>antiMarge-10mer_h2_pos23</t>
+  </si>
+  <si>
+    <t>antiLisa-10mer_h2_pos26</t>
+  </si>
+  <si>
+    <t>antiKrusty-10mer_h2_pos29</t>
+  </si>
+  <si>
+    <t>antiHomer-10mer_h2_pos32</t>
+  </si>
+  <si>
+    <t>Homer-10mer_h5_pos1</t>
+  </si>
+  <si>
+    <t>Krusty-10mer_h5_pos6</t>
+  </si>
+  <si>
+    <t>Lisa-10mer_h5_pos11</t>
+  </si>
+  <si>
+    <t>Marge-10mer_h5_pos16</t>
+  </si>
+  <si>
+    <t>Patty-10mer_h5_pos21</t>
+  </si>
+  <si>
+    <t>Quimby-10mer_h5_pos26</t>
+  </si>
+  <si>
+    <t>Smithers-10mer_h5_pos31</t>
+  </si>
+  <si>
+    <t>name-side-position</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1216,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1308,34 +1308,34 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
@@ -1357,34 +1357,34 @@
         <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -1406,7 +1406,7 @@
         <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>147</v>
@@ -1418,34 +1418,34 @@
         <v>149</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1463,25 +1463,25 @@
         <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -1506,7 +1506,7 @@
         <v>69</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>166</v>
+        <v>125</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>

</xml_diff>

<commit_message>
Put new standard-form cargo plates in cargo_plate folder
</commit_message>
<xml_diff>
--- a/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
+++ b/GUI/used-cargo-plates/P3518_MA_octahedron_patterning_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02764c23b0b97413/Cloud_Documents/Shih_Lab_2024/Crisscross-Design/GUI/used-cargo-plates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B5C4674-00C8-4EAA-B4F3-BD5F2D2EA9FE}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_9E0D8840CB2F072F731B3185651BC01676460B67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34CE8B7F-5089-4AA2-8357-C382DB49AC02}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
     <t>Smithers-10mer_h5_pos31</t>
   </si>
   <si>
-    <t>name-side-position</t>
+    <t>name_side_position</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1216,7 @@
   <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>